<commit_message>
changed century/daycent to century-daycent to avoid errors in web creation
</commit_message>
<xml_diff>
--- a/ProcessBasedModelsDatabase.xlsx
+++ b/ProcessBasedModelsDatabase.xlsx
@@ -2191,7 +2191,7 @@
     <t xml:space="preserve">DNDC is a computer simulation model of carbon and nitrogen biogeochemistry in agro-ecosystems. The model can be used for predicting crop growth, soil temperature and moisture regimes, soil carbon dynamics, nitrogen leaching, and emissions of trace gases including nitrous oxide (N2O), nitric oxide (NO), dinitrogen (N2), ammonia (NH3), methane (CH4) and carbon dioxide (CO2).  </t>
   </si>
   <si>
-    <t xml:space="preserve">CENTURY/DAYCENT</t>
+    <t xml:space="preserve">CENTURY-DAYCENT</t>
   </si>
   <si>
     <t xml:space="preserve">https://doi.org/10.1029/93GB02042</t>
@@ -3500,7 +3500,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;VERDADERO&quot;;&quot;VERDADERO&quot;;&quot;FALSO&quot;"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="9">
@@ -3984,14 +3984,14 @@
   <dimension ref="A1:CK194"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="J155" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D64" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A155" activeCellId="0" sqref="A155"/>
-      <selection pane="bottomRight" activeCell="L192" activeCellId="0" sqref="L192"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A64" activeCellId="0" sqref="A64"/>
+      <selection pane="bottomRight" activeCell="C111" activeCellId="0" sqref="C111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
@@ -4005,7 +4005,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="53.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="18.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="50.29"/>
@@ -4015,10 +4015,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="23.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="18.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="19.99"/>
@@ -4026,10 +4026,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="3" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="2" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="4" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="2" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="21.86"/>
@@ -4039,10 +4039,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="2" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="6" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="2" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="0" width="16.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="0" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="7" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="10.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="88" min="88" style="0" width="12.71"/>
   </cols>
   <sheetData>
@@ -4453,7 +4453,8 @@
         <v>107</v>
       </c>
       <c r="K3" s="16"/>
-      <c r="L3" s="34" t="b">
+      <c r="L3" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="T3" s="0" t="s">
@@ -4540,7 +4541,8 @@
         <v>107</v>
       </c>
       <c r="K4" s="16"/>
-      <c r="L4" s="34" t="b">
+      <c r="L4" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="T4" s="0" t="s">
@@ -4624,7 +4626,8 @@
         <v>119</v>
       </c>
       <c r="K5" s="16"/>
-      <c r="L5" s="34" t="b">
+      <c r="L5" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P5" s="36" t="s">
@@ -4714,7 +4717,8 @@
         <v>107</v>
       </c>
       <c r="K6" s="16"/>
-      <c r="L6" s="34" t="b">
+      <c r="L6" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M6" s="2" t="s">
@@ -4806,7 +4810,8 @@
         <v>130</v>
       </c>
       <c r="K7" s="16"/>
-      <c r="L7" s="34" t="b">
+      <c r="L7" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="O7" s="0" t="s">
@@ -4890,7 +4895,8 @@
       <c r="K8" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="L8" s="40" t="b">
+      <c r="L8" s="40" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -5004,7 +5010,8 @@
         <v>107</v>
       </c>
       <c r="K9" s="37"/>
-      <c r="L9" s="40" t="b">
+      <c r="L9" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N9" s="0" t="s">
@@ -5095,7 +5102,8 @@
         <v>107</v>
       </c>
       <c r="K10" s="37"/>
-      <c r="L10" s="40" t="b">
+      <c r="L10" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P10" s="36"/>
@@ -5183,7 +5191,8 @@
         <v>159</v>
       </c>
       <c r="K11" s="37"/>
-      <c r="L11" s="40" t="b">
+      <c r="L11" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P11" s="36"/>
@@ -5262,7 +5271,8 @@
         <v>165</v>
       </c>
       <c r="K12" s="37"/>
-      <c r="L12" s="40" t="b">
+      <c r="L12" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="O12" s="41"/>
@@ -5345,7 +5355,8 @@
         <v>107</v>
       </c>
       <c r="K13" s="37"/>
-      <c r="L13" s="40" t="b">
+      <c r="L13" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M13" s="2" t="s">
@@ -5439,7 +5450,8 @@
         <v>165</v>
       </c>
       <c r="K14" s="37"/>
-      <c r="L14" s="40" t="b">
+      <c r="L14" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M14" s="2" t="s">
@@ -5560,7 +5572,8 @@
         <v>165</v>
       </c>
       <c r="K15" s="37"/>
-      <c r="L15" s="40" t="b">
+      <c r="L15" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N15" s="42"/>
@@ -5660,7 +5673,8 @@
       <c r="K16" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="L16" s="40" t="b">
+      <c r="L16" s="40" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="O16" s="0" t="s">
@@ -5771,7 +5785,8 @@
         <v>107</v>
       </c>
       <c r="K17" s="37"/>
-      <c r="L17" s="40" t="b">
+      <c r="L17" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N17" s="0" t="s">
@@ -5887,7 +5902,8 @@
         <v>185</v>
       </c>
       <c r="K18" s="37"/>
-      <c r="L18" s="40" t="b">
+      <c r="L18" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -6002,7 +6018,8 @@
         <v>107</v>
       </c>
       <c r="K19" s="37"/>
-      <c r="L19" s="40" t="b">
+      <c r="L19" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P19" s="36"/>
@@ -6108,7 +6125,8 @@
         <v>209</v>
       </c>
       <c r="K20" s="37"/>
-      <c r="L20" s="40" t="b">
+      <c r="L20" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M20" s="2" t="s">
@@ -6230,7 +6248,8 @@
         <v>216</v>
       </c>
       <c r="K21" s="13"/>
-      <c r="L21" s="44" t="b">
+      <c r="L21" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="O21" s="41"/>
@@ -6328,7 +6347,8 @@
         <v>107</v>
       </c>
       <c r="K22" s="13"/>
-      <c r="L22" s="44" t="b">
+      <c r="L22" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="O22" s="41"/>
@@ -6413,7 +6433,8 @@
       <c r="K23" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="L23" s="48" t="b">
+      <c r="L23" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M23" s="2" t="s">
@@ -6526,7 +6547,8 @@
         <v>165</v>
       </c>
       <c r="K24" s="45"/>
-      <c r="L24" s="48" t="b">
+      <c r="L24" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M24" s="2" t="s">
@@ -6673,7 +6695,8 @@
         <v>107</v>
       </c>
       <c r="K25" s="45"/>
-      <c r="L25" s="48" t="b">
+      <c r="L25" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M25" s="2" t="s">
@@ -6789,7 +6812,8 @@
         <v>107</v>
       </c>
       <c r="K26" s="45"/>
-      <c r="L26" s="48" t="b">
+      <c r="L26" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M26" s="2" t="s">
@@ -6915,7 +6939,8 @@
         <v>165</v>
       </c>
       <c r="K27" s="45"/>
-      <c r="L27" s="48" t="b">
+      <c r="L27" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N27" s="0" t="s">
@@ -7044,7 +7069,8 @@
       <c r="K28" s="45" t="s">
         <v>254</v>
       </c>
-      <c r="L28" s="48" t="b">
+      <c r="L28" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="O28" s="0" t="s">
@@ -7181,7 +7207,8 @@
       <c r="K29" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="L29" s="48" t="b">
+      <c r="L29" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N29" s="0" t="s">
@@ -7325,7 +7352,8 @@
         <v>216</v>
       </c>
       <c r="K30" s="45"/>
-      <c r="L30" s="48" t="b">
+      <c r="L30" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P30" s="36" t="s">
@@ -7452,7 +7480,8 @@
         <v>165</v>
       </c>
       <c r="K31" s="45"/>
-      <c r="L31" s="48" t="b">
+      <c r="L31" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M31" s="2" t="s">
@@ -7586,7 +7615,8 @@
       <c r="K32" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="L32" s="48" t="b">
+      <c r="L32" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N32" s="0" t="s">
@@ -7729,7 +7759,8 @@
       <c r="K33" s="45" t="s">
         <v>287</v>
       </c>
-      <c r="L33" s="48" t="b">
+      <c r="L33" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N33" s="0" t="s">
@@ -7861,7 +7892,8 @@
         <v>296</v>
       </c>
       <c r="K34" s="45"/>
-      <c r="L34" s="48" t="b">
+      <c r="L34" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N34" s="42"/>
@@ -8000,7 +8032,8 @@
       <c r="K35" s="45" t="s">
         <v>303</v>
       </c>
-      <c r="L35" s="48" t="b">
+      <c r="L35" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M35" s="2" t="s">
@@ -8148,7 +8181,8 @@
         <v>107</v>
       </c>
       <c r="K36" s="45"/>
-      <c r="L36" s="48" t="b">
+      <c r="L36" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M36" s="2" t="s">
@@ -8299,7 +8333,8 @@
         <v>315</v>
       </c>
       <c r="K37" s="45"/>
-      <c r="L37" s="48" t="b">
+      <c r="L37" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M37" s="2" t="s">
@@ -8444,7 +8479,8 @@
         <v>315</v>
       </c>
       <c r="K38" s="45"/>
-      <c r="L38" s="48" t="b">
+      <c r="L38" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M38" s="2" t="s">
@@ -8560,7 +8596,8 @@
         <v>315</v>
       </c>
       <c r="K39" s="45"/>
-      <c r="L39" s="48" t="b">
+      <c r="L39" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N39" s="42"/>
@@ -8684,7 +8721,8 @@
         <v>107</v>
       </c>
       <c r="K40" s="45"/>
-      <c r="L40" s="48" t="b">
+      <c r="L40" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N40" s="42"/>
@@ -8799,7 +8837,8 @@
         <v>130</v>
       </c>
       <c r="K41" s="45"/>
-      <c r="L41" s="48" t="b">
+      <c r="L41" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M41" s="2" t="s">
@@ -8942,7 +8981,8 @@
         <v>315</v>
       </c>
       <c r="K42" s="45"/>
-      <c r="L42" s="48" t="b">
+      <c r="L42" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M42" s="2" t="s">
@@ -9079,7 +9119,8 @@
         <v>165</v>
       </c>
       <c r="K43" s="45"/>
-      <c r="L43" s="48" t="b">
+      <c r="L43" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M43" s="2" t="s">
@@ -9216,7 +9257,8 @@
         <v>107</v>
       </c>
       <c r="K44" s="45"/>
-      <c r="L44" s="48" t="b">
+      <c r="L44" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N44" s="42"/>
@@ -9350,7 +9392,8 @@
       <c r="K45" s="45" t="s">
         <v>357</v>
       </c>
-      <c r="L45" s="48" t="b">
+      <c r="L45" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M45" s="2" t="s">
@@ -9494,7 +9537,8 @@
         <v>315</v>
       </c>
       <c r="K46" s="45"/>
-      <c r="L46" s="48" t="b">
+      <c r="L46" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M46" s="2" t="s">
@@ -9615,7 +9659,8 @@
         <v>185</v>
       </c>
       <c r="K47" s="45"/>
-      <c r="L47" s="48" t="b">
+      <c r="L47" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M47" s="2" t="s">
@@ -9748,7 +9793,8 @@
         <v>107</v>
       </c>
       <c r="K48" s="45"/>
-      <c r="L48" s="48" t="b">
+      <c r="L48" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M48" s="2" t="s">
@@ -9888,7 +9934,8 @@
       <c r="K49" s="45" t="s">
         <v>385</v>
       </c>
-      <c r="L49" s="48" t="b">
+      <c r="L49" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M49" s="2" t="s">
@@ -10046,7 +10093,8 @@
       <c r="K50" s="45" t="s">
         <v>394</v>
       </c>
-      <c r="L50" s="48" t="b">
+      <c r="L50" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M50" s="2" t="s">
@@ -10187,7 +10235,8 @@
         <v>130</v>
       </c>
       <c r="K51" s="45"/>
-      <c r="L51" s="48" t="b">
+      <c r="L51" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M51" s="2" t="s">
@@ -10328,7 +10377,8 @@
         <v>209</v>
       </c>
       <c r="K52" s="45"/>
-      <c r="L52" s="48" t="b">
+      <c r="L52" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N52" s="0" t="s">
@@ -10456,7 +10506,8 @@
         <v>185</v>
       </c>
       <c r="K53" s="45"/>
-      <c r="L53" s="48" t="b">
+      <c r="L53" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M53" s="2" t="s">
@@ -10601,7 +10652,8 @@
         <v>130</v>
       </c>
       <c r="K54" s="45"/>
-      <c r="L54" s="48" t="b">
+      <c r="L54" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M54" s="2" t="s">
@@ -10739,7 +10791,8 @@
         <v>107</v>
       </c>
       <c r="K55" s="45"/>
-      <c r="L55" s="48" t="b">
+      <c r="L55" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M55" s="2" t="s">
@@ -10885,7 +10938,8 @@
       <c r="K56" s="45" t="s">
         <v>423</v>
       </c>
-      <c r="L56" s="48" t="b">
+      <c r="L56" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N56" s="0" t="s">
@@ -11044,7 +11098,8 @@
         <v>431</v>
       </c>
       <c r="K57" s="45"/>
-      <c r="L57" s="48" t="b">
+      <c r="L57" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M57" s="2" t="s">
@@ -11186,7 +11241,8 @@
         <v>165</v>
       </c>
       <c r="K58" s="45"/>
-      <c r="L58" s="48" t="b">
+      <c r="L58" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M58" s="2" t="s">
@@ -11324,7 +11380,8 @@
       <c r="K59" s="45" t="s">
         <v>440</v>
       </c>
-      <c r="L59" s="48" t="b">
+      <c r="L59" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M59" s="2" t="s">
@@ -11471,7 +11528,8 @@
         <v>107</v>
       </c>
       <c r="K60" s="45"/>
-      <c r="L60" s="48" t="b">
+      <c r="L60" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M60" s="2" t="s">
@@ -11627,7 +11685,8 @@
       <c r="K61" s="16" t="s">
         <v>456</v>
       </c>
-      <c r="L61" s="34" t="b">
+      <c r="L61" s="34" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="O61" s="41"/>
@@ -11710,7 +11769,8 @@
         <v>119</v>
       </c>
       <c r="K62" s="16"/>
-      <c r="L62" s="34" t="b">
+      <c r="L62" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="O62" s="41"/>
@@ -11796,7 +11856,8 @@
         <v>130</v>
       </c>
       <c r="K63" s="16"/>
-      <c r="L63" s="34" t="b">
+      <c r="L63" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="O63" s="41"/>
@@ -11893,7 +11954,8 @@
         <v>165</v>
       </c>
       <c r="K64" s="16"/>
-      <c r="L64" s="34" t="b">
+      <c r="L64" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P64" s="36"/>
@@ -11975,7 +12037,8 @@
         <v>479</v>
       </c>
       <c r="K65" s="16"/>
-      <c r="L65" s="34" t="b">
+      <c r="L65" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N65" s="41"/>
@@ -12058,7 +12121,8 @@
       <c r="K66" s="16" t="s">
         <v>484</v>
       </c>
-      <c r="L66" s="34" t="b">
+      <c r="L66" s="34" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P66" s="36" t="s">
@@ -12134,7 +12198,8 @@
         <v>107</v>
       </c>
       <c r="K67" s="16"/>
-      <c r="L67" s="34" t="b">
+      <c r="L67" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P67" s="36"/>
@@ -12216,7 +12281,8 @@
         <v>130</v>
       </c>
       <c r="K68" s="16"/>
-      <c r="L68" s="34" t="b">
+      <c r="L68" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P68" s="36"/>
@@ -12298,7 +12364,8 @@
         <v>431</v>
       </c>
       <c r="K69" s="16"/>
-      <c r="L69" s="34" t="b">
+      <c r="L69" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P69" s="36"/>
@@ -12378,7 +12445,8 @@
         <v>119</v>
       </c>
       <c r="K70" s="16"/>
-      <c r="L70" s="34" t="b">
+      <c r="L70" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P70" s="36"/>
@@ -12508,7 +12576,8 @@
       <c r="K71" s="16" t="s">
         <v>506</v>
       </c>
-      <c r="L71" s="34" t="b">
+      <c r="L71" s="34" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P71" s="36" t="s">
@@ -12598,7 +12667,8 @@
       <c r="K72" s="16" t="s">
         <v>512</v>
       </c>
-      <c r="L72" s="34" t="b">
+      <c r="L72" s="34" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P72" s="36" t="s">
@@ -12688,7 +12758,8 @@
       <c r="K73" s="16" t="s">
         <v>518</v>
       </c>
-      <c r="L73" s="34" t="b">
+      <c r="L73" s="34" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P73" s="36" t="s">
@@ -12779,7 +12850,8 @@
         <v>159</v>
       </c>
       <c r="K74" s="16"/>
-      <c r="L74" s="34" t="b">
+      <c r="L74" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P74" s="36"/>
@@ -12870,7 +12942,8 @@
         <v>107</v>
       </c>
       <c r="K75" s="16"/>
-      <c r="L75" s="34" t="b">
+      <c r="L75" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P75" s="36" t="s">
@@ -12970,7 +13043,8 @@
         <v>185</v>
       </c>
       <c r="K76" s="16"/>
-      <c r="L76" s="34" t="b">
+      <c r="L76" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N76" s="0" t="s">
@@ -13079,7 +13153,8 @@
         <v>479</v>
       </c>
       <c r="K77" s="16"/>
-      <c r="L77" s="34" t="b">
+      <c r="L77" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="O77" s="41"/>
@@ -13184,7 +13259,8 @@
         <v>547</v>
       </c>
       <c r="K78" s="16"/>
-      <c r="L78" s="34" t="b">
+      <c r="L78" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M78" s="2" t="s">
@@ -13284,7 +13360,8 @@
         <v>107</v>
       </c>
       <c r="K79" s="16"/>
-      <c r="L79" s="34" t="b">
+      <c r="L79" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P79" s="36"/>
@@ -13373,7 +13450,8 @@
         <v>547</v>
       </c>
       <c r="K80" s="16"/>
-      <c r="L80" s="34" t="b">
+      <c r="L80" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M80" s="2" t="s">
@@ -13496,7 +13574,8 @@
         <v>107</v>
       </c>
       <c r="K81" s="37"/>
-      <c r="L81" s="40" t="b">
+      <c r="L81" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P81" s="36"/>
@@ -13594,7 +13673,8 @@
         <v>185</v>
       </c>
       <c r="K82" s="37"/>
-      <c r="L82" s="40" t="b">
+      <c r="L82" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="O82" s="41"/>
@@ -13681,7 +13761,8 @@
         <v>107</v>
       </c>
       <c r="K83" s="37"/>
-      <c r="L83" s="40" t="b">
+      <c r="L83" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N83" s="0" t="s">
@@ -13782,7 +13863,8 @@
         <v>107</v>
       </c>
       <c r="K84" s="37"/>
-      <c r="L84" s="40" t="b">
+      <c r="L84" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="O84" s="41"/>
@@ -13871,7 +13953,8 @@
         <v>165</v>
       </c>
       <c r="K85" s="37"/>
-      <c r="L85" s="40" t="b">
+      <c r="L85" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="O85" s="41"/>
@@ -13984,7 +14067,8 @@
         <v>119</v>
       </c>
       <c r="K86" s="37"/>
-      <c r="L86" s="40" t="b">
+      <c r="L86" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P86" s="36" t="s">
@@ -14102,7 +14186,8 @@
         <v>107</v>
       </c>
       <c r="K87" s="37"/>
-      <c r="L87" s="40" t="b">
+      <c r="L87" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P87" s="36"/>
@@ -14199,7 +14284,8 @@
         <v>185</v>
       </c>
       <c r="K88" s="37"/>
-      <c r="L88" s="40" t="b">
+      <c r="L88" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N88" s="0" t="s">
@@ -14309,7 +14395,8 @@
         <v>600</v>
       </c>
       <c r="K89" s="37"/>
-      <c r="L89" s="40" t="b">
+      <c r="L89" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P89" s="36"/>
@@ -14397,7 +14484,8 @@
         <v>119</v>
       </c>
       <c r="K90" s="37"/>
-      <c r="L90" s="40" t="b">
+      <c r="L90" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N90" s="0" t="s">
@@ -14525,7 +14613,8 @@
         <v>315</v>
       </c>
       <c r="K91" s="37"/>
-      <c r="L91" s="40" t="b">
+      <c r="L91" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P91" s="36"/>
@@ -14638,7 +14727,8 @@
         <v>107</v>
       </c>
       <c r="K92" s="37"/>
-      <c r="L92" s="40" t="b">
+      <c r="L92" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M92" s="2" t="s">
@@ -14742,7 +14832,8 @@
       <c r="K93" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="L93" s="40" t="b">
+      <c r="L93" s="40" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N93" s="41"/>
@@ -14847,7 +14938,8 @@
       <c r="K94" s="37" t="s">
         <v>628</v>
       </c>
-      <c r="L94" s="40" t="b">
+      <c r="L94" s="40" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N94" s="0" t="s">
@@ -14980,7 +15072,8 @@
         <v>600</v>
       </c>
       <c r="K95" s="37"/>
-      <c r="L95" s="40" t="b">
+      <c r="L95" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M95" s="2" t="s">
@@ -15084,7 +15177,8 @@
         <v>315</v>
       </c>
       <c r="K96" s="37"/>
-      <c r="L96" s="40" t="b">
+      <c r="L96" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N96" s="0" t="s">
@@ -15210,7 +15304,8 @@
         <v>547</v>
       </c>
       <c r="K97" s="37"/>
-      <c r="L97" s="40" t="b">
+      <c r="L97" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P97" s="36" t="s">
@@ -15343,7 +15438,8 @@
         <v>119</v>
       </c>
       <c r="K98" s="37"/>
-      <c r="L98" s="40" t="b">
+      <c r="L98" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N98" s="0" t="s">
@@ -15464,7 +15560,8 @@
         <v>185</v>
       </c>
       <c r="K99" s="37"/>
-      <c r="L99" s="40" t="b">
+      <c r="L99" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N99" s="0" t="s">
@@ -15592,7 +15689,8 @@
         <v>660</v>
       </c>
       <c r="K100" s="37"/>
-      <c r="L100" s="40" t="b">
+      <c r="L100" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N100" s="0" t="s">
@@ -15692,7 +15790,8 @@
         <v>165</v>
       </c>
       <c r="K101" s="37"/>
-      <c r="L101" s="40" t="b">
+      <c r="L101" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P101" s="49" t="s">
@@ -15791,7 +15890,8 @@
       <c r="K102" s="37" t="s">
         <v>672</v>
       </c>
-      <c r="L102" s="40" t="b">
+      <c r="L102" s="40" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P102" s="36" t="s">
@@ -15921,7 +16021,8 @@
         <v>315</v>
       </c>
       <c r="K103" s="37"/>
-      <c r="L103" s="40" t="b">
+      <c r="L103" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N103" s="0" t="s">
@@ -16041,7 +16142,8 @@
         <v>107</v>
       </c>
       <c r="K104" s="37"/>
-      <c r="L104" s="40" t="b">
+      <c r="L104" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="O104" s="0" t="s">
@@ -16135,7 +16237,8 @@
         <v>130</v>
       </c>
       <c r="K105" s="37"/>
-      <c r="L105" s="40" t="b">
+      <c r="L105" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M105" s="2" t="s">
@@ -16262,7 +16365,8 @@
         <v>107</v>
       </c>
       <c r="K106" s="37"/>
-      <c r="L106" s="40" t="b">
+      <c r="L106" s="40" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M106" s="2" t="s">
@@ -16362,7 +16466,8 @@
       <c r="K107" s="37" t="s">
         <v>701</v>
       </c>
-      <c r="L107" s="40" t="b">
+      <c r="L107" s="40" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N107" s="0" t="s">
@@ -16466,7 +16571,8 @@
       <c r="K108" s="37" t="s">
         <v>709</v>
       </c>
-      <c r="L108" s="40" t="b">
+      <c r="L108" s="40" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N108" s="0" t="s">
@@ -16561,7 +16667,8 @@
         <v>107</v>
       </c>
       <c r="K109" s="50"/>
-      <c r="L109" s="53" t="b">
+      <c r="L109" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P109" s="36"/>
@@ -16642,7 +16749,8 @@
       <c r="K110" s="50" t="s">
         <v>722</v>
       </c>
-      <c r="L110" s="53" t="b">
+      <c r="L110" s="53" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P110" s="36" t="s">
@@ -16735,7 +16843,8 @@
       <c r="K111" s="50" t="s">
         <v>727</v>
       </c>
-      <c r="L111" s="53" t="b">
+      <c r="L111" s="53" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P111" s="36" t="s">
@@ -16853,7 +16962,8 @@
         <v>165</v>
       </c>
       <c r="K112" s="50"/>
-      <c r="L112" s="53" t="b">
+      <c r="L112" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P112" s="36" t="s">
@@ -16951,7 +17061,8 @@
       <c r="K113" s="50" t="s">
         <v>739</v>
       </c>
-      <c r="L113" s="53" t="b">
+      <c r="L113" s="53" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P113" s="36" t="s">
@@ -17052,7 +17163,8 @@
       <c r="K114" s="50" t="s">
         <v>747</v>
       </c>
-      <c r="L114" s="53" t="b">
+      <c r="L114" s="53" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P114" s="36" t="s">
@@ -17127,7 +17239,8 @@
         <v>165</v>
       </c>
       <c r="K115" s="50"/>
-      <c r="L115" s="53" t="b">
+      <c r="L115" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M115" s="2" t="s">
@@ -17223,7 +17336,8 @@
         <v>107</v>
       </c>
       <c r="K116" s="50"/>
-      <c r="L116" s="53" t="b">
+      <c r="L116" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P116" s="36"/>
@@ -17296,7 +17410,8 @@
         <v>107</v>
       </c>
       <c r="K117" s="50"/>
-      <c r="L117" s="53" t="b">
+      <c r="L117" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P117" s="36"/>
@@ -17369,7 +17484,8 @@
         <v>107</v>
       </c>
       <c r="K118" s="50"/>
-      <c r="L118" s="53" t="b">
+      <c r="L118" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P118" s="36"/>
@@ -17442,7 +17558,8 @@
         <v>315</v>
       </c>
       <c r="K119" s="50"/>
-      <c r="L119" s="53" t="b">
+      <c r="L119" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P119" s="36"/>
@@ -17518,7 +17635,8 @@
         <v>107</v>
       </c>
       <c r="K120" s="50"/>
-      <c r="L120" s="53" t="b">
+      <c r="L120" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P120" s="36"/>
@@ -17588,7 +17706,8 @@
         <v>107</v>
       </c>
       <c r="K121" s="50"/>
-      <c r="L121" s="53" t="b">
+      <c r="L121" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M121" s="2" t="s">
@@ -17672,7 +17791,8 @@
       <c r="K122" s="50" t="s">
         <v>790</v>
       </c>
-      <c r="L122" s="53" t="b">
+      <c r="L122" s="53" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P122" s="36" t="s">
@@ -17747,7 +17867,8 @@
         <v>107</v>
       </c>
       <c r="K123" s="50"/>
-      <c r="L123" s="53" t="b">
+      <c r="L123" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M123" s="2" t="s">
@@ -17831,7 +17952,8 @@
         <v>107</v>
       </c>
       <c r="K124" s="50"/>
-      <c r="L124" s="53" t="b">
+      <c r="L124" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M124" s="2" t="s">
@@ -17908,7 +18030,8 @@
         <v>107</v>
       </c>
       <c r="K125" s="50"/>
-      <c r="L125" s="53" t="b">
+      <c r="L125" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P125" s="36"/>
@@ -17987,7 +18110,8 @@
         <v>315</v>
       </c>
       <c r="K126" s="50"/>
-      <c r="L126" s="53" t="b">
+      <c r="L126" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M126" s="2" t="s">
@@ -18081,7 +18205,8 @@
       <c r="K127" s="50" t="s">
         <v>812</v>
       </c>
-      <c r="L127" s="53" t="b">
+      <c r="L127" s="53" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P127" s="36" t="s">
@@ -18171,7 +18296,8 @@
         <v>107</v>
       </c>
       <c r="K128" s="50"/>
-      <c r="L128" s="53" t="b">
+      <c r="L128" s="53" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M128" s="2" t="s">
@@ -18267,7 +18393,8 @@
       <c r="K129" s="13" t="s">
         <v>826</v>
       </c>
-      <c r="L129" s="44" t="b">
+      <c r="L129" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N129" s="41"/>
@@ -18352,7 +18479,8 @@
       <c r="K130" s="13" t="s">
         <v>831</v>
       </c>
-      <c r="L130" s="44" t="b">
+      <c r="L130" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M130" s="2" t="s">
@@ -18470,7 +18598,8 @@
         <v>431</v>
       </c>
       <c r="K131" s="13"/>
-      <c r="L131" s="44" t="b">
+      <c r="L131" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N131" s="41"/>
@@ -18563,7 +18692,8 @@
         <v>107</v>
       </c>
       <c r="K132" s="13"/>
-      <c r="L132" s="44" t="b">
+      <c r="L132" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M132" s="2" t="s">
@@ -18656,7 +18786,8 @@
         <v>107</v>
       </c>
       <c r="K133" s="13"/>
-      <c r="L133" s="44" t="b">
+      <c r="L133" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M133" s="2" t="s">
@@ -18749,7 +18880,8 @@
         <v>216</v>
       </c>
       <c r="K134" s="13"/>
-      <c r="L134" s="44" t="b">
+      <c r="L134" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N134" s="41"/>
@@ -18844,7 +18976,8 @@
       <c r="K135" s="13" t="s">
         <v>854</v>
       </c>
-      <c r="L135" s="44" t="b">
+      <c r="L135" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P135" s="36" t="s">
@@ -18931,7 +19064,8 @@
       <c r="K136" s="54" t="s">
         <v>860</v>
       </c>
-      <c r="L136" s="44" t="b">
+      <c r="L136" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M136" s="2" t="s">
@@ -19049,7 +19183,8 @@
         <v>119</v>
       </c>
       <c r="K137" s="13"/>
-      <c r="L137" s="44" t="b">
+      <c r="L137" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M137" s="2" t="s">
@@ -19150,7 +19285,8 @@
         <v>315</v>
       </c>
       <c r="K138" s="13"/>
-      <c r="L138" s="44" t="b">
+      <c r="L138" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P138" s="36"/>
@@ -19230,7 +19366,8 @@
         <v>107</v>
       </c>
       <c r="K139" s="13"/>
-      <c r="L139" s="44" t="b">
+      <c r="L139" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M139" s="2" t="s">
@@ -19355,7 +19492,8 @@
       <c r="K140" s="13" t="s">
         <v>880</v>
       </c>
-      <c r="L140" s="44" t="b">
+      <c r="L140" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P140" s="36" t="s">
@@ -19452,7 +19590,8 @@
         <v>209</v>
       </c>
       <c r="K141" s="13"/>
-      <c r="L141" s="44" t="b">
+      <c r="L141" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P141" s="36"/>
@@ -19558,7 +19697,8 @@
         <v>891</v>
       </c>
       <c r="K142" s="13"/>
-      <c r="L142" s="44" t="b">
+      <c r="L142" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M142" s="2" t="s">
@@ -19668,7 +19808,8 @@
         <v>107</v>
       </c>
       <c r="K143" s="13"/>
-      <c r="L143" s="44" t="b">
+      <c r="L143" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M143" s="2" t="s">
@@ -19789,7 +19930,8 @@
         <v>107</v>
       </c>
       <c r="K144" s="13"/>
-      <c r="L144" s="44" t="b">
+      <c r="L144" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M144" s="2" t="s">
@@ -19911,7 +20053,8 @@
         <v>107</v>
       </c>
       <c r="K145" s="13"/>
-      <c r="L145" s="44" t="b">
+      <c r="L145" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M145" s="2" t="s">
@@ -20009,7 +20152,8 @@
       <c r="K146" s="13" t="s">
         <v>907</v>
       </c>
-      <c r="L146" s="44" t="b">
+      <c r="L146" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M146" s="2" t="s">
@@ -20138,7 +20282,8 @@
         <v>130</v>
       </c>
       <c r="K147" s="13"/>
-      <c r="L147" s="44" t="b">
+      <c r="L147" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M147" s="2" t="s">
@@ -20256,7 +20401,8 @@
         <v>107</v>
       </c>
       <c r="K148" s="45"/>
-      <c r="L148" s="48" t="b">
+      <c r="L148" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N148" s="0" t="s">
@@ -20381,7 +20527,8 @@
         <v>479</v>
       </c>
       <c r="K149" s="45"/>
-      <c r="L149" s="48" t="b">
+      <c r="L149" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P149" s="36"/>
@@ -20515,7 +20662,8 @@
         <v>165</v>
       </c>
       <c r="K150" s="45"/>
-      <c r="L150" s="48" t="b">
+      <c r="L150" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M150" s="2" t="s">
@@ -20627,7 +20775,8 @@
       <c r="K151" s="45" t="s">
         <v>932</v>
       </c>
-      <c r="L151" s="48" t="b">
+      <c r="L151" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M151" s="2" t="s">
@@ -20727,7 +20876,8 @@
         <v>315</v>
       </c>
       <c r="K152" s="45"/>
-      <c r="L152" s="48" t="b">
+      <c r="L152" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P152" s="36" t="s">
@@ -20826,7 +20976,8 @@
         <v>600</v>
       </c>
       <c r="K153" s="45"/>
-      <c r="L153" s="48" t="b">
+      <c r="L153" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P153" s="36"/>
@@ -20921,7 +21072,8 @@
         <v>315</v>
       </c>
       <c r="K154" s="45"/>
-      <c r="L154" s="48" t="b">
+      <c r="L154" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P154" s="36"/>
@@ -21049,7 +21201,8 @@
         <v>107</v>
       </c>
       <c r="K155" s="45"/>
-      <c r="L155" s="48" t="b">
+      <c r="L155" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P155" s="36"/>
@@ -21157,7 +21310,8 @@
       <c r="K156" s="45" t="s">
         <v>957</v>
       </c>
-      <c r="L156" s="48" t="b">
+      <c r="L156" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P156" s="36" t="s">
@@ -21298,7 +21452,8 @@
         <v>600</v>
       </c>
       <c r="K157" s="45"/>
-      <c r="L157" s="48" t="b">
+      <c r="L157" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P157" s="36" t="s">
@@ -21400,7 +21555,8 @@
         <v>159</v>
       </c>
       <c r="K158" s="45"/>
-      <c r="L158" s="48" t="b">
+      <c r="L158" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P158" s="36"/>
@@ -21556,7 +21712,8 @@
       <c r="K159" s="45" t="s">
         <v>974</v>
       </c>
-      <c r="L159" s="48" t="b">
+      <c r="L159" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P159" s="36" t="s">
@@ -21667,7 +21824,8 @@
         <v>165</v>
       </c>
       <c r="K160" s="45"/>
-      <c r="L160" s="48" t="b">
+      <c r="L160" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P160" s="36"/>
@@ -21767,7 +21925,8 @@
         <v>165</v>
       </c>
       <c r="K161" s="45"/>
-      <c r="L161" s="48" t="b">
+      <c r="L161" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P161" s="36"/>
@@ -21867,7 +22026,8 @@
         <v>130</v>
       </c>
       <c r="K162" s="45"/>
-      <c r="L162" s="48" t="b">
+      <c r="L162" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M162" s="2" t="s">
@@ -22010,7 +22170,8 @@
         <v>130</v>
       </c>
       <c r="K163" s="45"/>
-      <c r="L163" s="48" t="b">
+      <c r="L163" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P163" s="36" t="s">
@@ -22124,7 +22285,8 @@
         <v>209</v>
       </c>
       <c r="K164" s="45"/>
-      <c r="L164" s="48" t="b">
+      <c r="L164" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N164" s="0" t="s">
@@ -22236,7 +22398,8 @@
         <v>660</v>
       </c>
       <c r="K165" s="45"/>
-      <c r="L165" s="48" t="b">
+      <c r="L165" s="48" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M165" s="2" t="s">
@@ -22367,7 +22530,8 @@
       <c r="K166" s="45" t="s">
         <v>1010</v>
       </c>
-      <c r="L166" s="48" t="b">
+      <c r="L166" s="48" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N166" s="0" t="s">
@@ -22494,7 +22658,8 @@
         <v>185</v>
       </c>
       <c r="K167" s="16"/>
-      <c r="L167" s="34" t="b">
+      <c r="L167" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P167" s="36"/>
@@ -22580,7 +22745,8 @@
         <v>185</v>
       </c>
       <c r="K168" s="16"/>
-      <c r="L168" s="34" t="b">
+      <c r="L168" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N168" s="55"/>
@@ -22677,7 +22843,8 @@
       <c r="K169" s="16" t="s">
         <v>1029</v>
       </c>
-      <c r="L169" s="34" t="b">
+      <c r="L169" s="34" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N169" s="0" t="s">
@@ -22822,7 +22989,8 @@
         <v>107</v>
       </c>
       <c r="K170" s="16"/>
-      <c r="L170" s="34" t="b">
+      <c r="L170" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N170" s="0" t="s">
@@ -22911,7 +23079,8 @@
         <v>107</v>
       </c>
       <c r="K171" s="16"/>
-      <c r="L171" s="34" t="b">
+      <c r="L171" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P171" s="36" t="s">
@@ -23038,7 +23207,8 @@
         <v>119</v>
       </c>
       <c r="K172" s="16"/>
-      <c r="L172" s="34" t="b">
+      <c r="L172" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M172" s="2" t="s">
@@ -23149,7 +23319,8 @@
         <v>119</v>
       </c>
       <c r="K173" s="16"/>
-      <c r="L173" s="34" t="b">
+      <c r="L173" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N173" s="0" t="s">
@@ -23261,7 +23432,8 @@
         <v>107</v>
       </c>
       <c r="K174" s="16"/>
-      <c r="L174" s="34" t="b">
+      <c r="L174" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P174" s="36" t="s">
@@ -23369,7 +23541,8 @@
         <v>431</v>
       </c>
       <c r="K175" s="16"/>
-      <c r="L175" s="34" t="b">
+      <c r="L175" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N175" s="0" t="s">
@@ -23511,7 +23684,8 @@
       <c r="K176" s="16" t="s">
         <v>1067</v>
       </c>
-      <c r="L176" s="34" t="b">
+      <c r="L176" s="34" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="P176" s="36" t="s">
@@ -23649,7 +23823,8 @@
       <c r="K177" s="16" t="s">
         <v>1070</v>
       </c>
-      <c r="L177" s="34" t="b">
+      <c r="L177" s="34" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N177" s="0" t="s">
@@ -23779,7 +23954,8 @@
         <v>315</v>
       </c>
       <c r="K178" s="16"/>
-      <c r="L178" s="34" t="b">
+      <c r="L178" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M178" s="2" t="s">
@@ -23915,7 +24091,8 @@
         <v>107</v>
       </c>
       <c r="K179" s="16"/>
-      <c r="L179" s="34" t="b">
+      <c r="L179" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M179" s="2" t="s">
@@ -24031,7 +24208,8 @@
         <v>209</v>
       </c>
       <c r="K180" s="16"/>
-      <c r="L180" s="34" t="b">
+      <c r="L180" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N180" s="0" t="s">
@@ -24126,7 +24304,8 @@
         <v>107</v>
       </c>
       <c r="K181" s="16"/>
-      <c r="L181" s="34" t="b">
+      <c r="L181" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N181" s="0" t="s">
@@ -24276,7 +24455,8 @@
         <v>431</v>
       </c>
       <c r="K182" s="16"/>
-      <c r="L182" s="34" t="b">
+      <c r="L182" s="34" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N182" s="0" t="s">
@@ -24394,7 +24574,8 @@
         <v>107</v>
       </c>
       <c r="K183" s="13"/>
-      <c r="L183" s="44" t="b">
+      <c r="L183" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P183" s="36"/>
@@ -24480,7 +24661,8 @@
         <v>107</v>
       </c>
       <c r="K184" s="13"/>
-      <c r="L184" s="44" t="b">
+      <c r="L184" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P184" s="36"/>
@@ -24569,7 +24751,8 @@
         <v>107</v>
       </c>
       <c r="K185" s="13"/>
-      <c r="L185" s="44" t="b">
+      <c r="L185" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="U185" s="0" t="s">
@@ -24666,7 +24849,8 @@
         <v>130</v>
       </c>
       <c r="K186" s="13"/>
-      <c r="L186" s="44" t="b">
+      <c r="L186" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="S186" s="2" t="s">
@@ -24790,7 +24974,8 @@
         <v>479</v>
       </c>
       <c r="K187" s="13"/>
-      <c r="L187" s="44" t="b">
+      <c r="L187" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="M187" s="2" t="s">
@@ -24895,7 +25080,8 @@
       <c r="K188" s="13" t="s">
         <v>1119</v>
       </c>
-      <c r="L188" s="44" t="b">
+      <c r="L188" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N188" s="0" t="s">
@@ -24997,7 +25183,8 @@
       <c r="K189" s="13" t="s">
         <v>1125</v>
       </c>
-      <c r="L189" s="44" t="b">
+      <c r="L189" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="O189" s="0" t="s">
@@ -25090,7 +25277,8 @@
       <c r="K190" s="13" t="s">
         <v>1131</v>
       </c>
-      <c r="L190" s="44" t="b">
+      <c r="L190" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M190" s="2" t="s">
@@ -25199,7 +25387,8 @@
         <v>107</v>
       </c>
       <c r="K191" s="13"/>
-      <c r="L191" s="44" t="b">
+      <c r="L191" s="44" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N191" s="55"/>
@@ -25316,7 +25505,8 @@
       <c r="K192" s="13" t="s">
         <v>1141</v>
       </c>
-      <c r="L192" s="44" t="b">
+      <c r="L192" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N192" s="55" t="s">
@@ -25480,7 +25670,8 @@
       <c r="K193" s="13" t="s">
         <v>1149</v>
       </c>
-      <c r="L193" s="44" t="b">
+      <c r="L193" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="N193" s="55"/>
@@ -25616,7 +25807,8 @@
       <c r="K194" s="13" t="s">
         <v>1155</v>
       </c>
-      <c r="L194" s="44" t="b">
+      <c r="L194" s="44" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M194" s="2" t="s">
@@ -25974,8 +26166,8 @@
     <hyperlink ref="P194" r:id="rId278" display="https://cafnrfaculty.missouri.edu/gislab/landis/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>